<commit_message>
Day4-first commit:The Website displays the list of Doctors matching the searched condition
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/inputData.xlsx
+++ b/src/test/resources/Exceldata/inputData.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4976A66A-8BEC-4A81-99BE-93C21684F9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMILE\Desktop\Apollo Testing\Apollo247TestingApp\src\test\resources\Exceldata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509C474E-2FF8-46FA-8E8A-1016F1F6BF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -341,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -359,7 +363,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>8667695616</v>
+        <v>9600794463</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>123456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day4-first commit:The automation successfully selected the doctor and view their details
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/inputData.xlsx
+++ b/src/test/resources/Exceldata/inputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMILE\Desktop\Apollo Testing\Apollo247TestingApp\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509C474E-2FF8-46FA-8E8A-1016F1F6BF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48890C7-7759-411F-9061-E1B497718B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,7 +363,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>9600794463</v>
+        <v>9791400550</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Day5-first commit:The automation successfully schedule the appointment for the doctor
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/inputData.xlsx
+++ b/src/test/resources/Exceldata/inputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMILE\Desktop\Apollo Testing\Apollo247TestingApp\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48890C7-7759-411F-9061-E1B497718B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACB805A-D103-482F-9D10-9DE33B2795B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -363,7 +363,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>9791400550</v>
+        <v>8667695616</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Day5-second commit The automation successfully add patient details for the appointment
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/inputData.xlsx
+++ b/src/test/resources/Exceldata/inputData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMILE\Desktop\Apollo Testing\Apollo247TestingApp\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACB805A-D103-482F-9D10-9DE33B2795B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1815D8-DE0B-4C85-A76B-FD2C85007E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2800" yWindow="2800" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,19 +25,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>abi</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>abi@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -60,13 +86,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -345,33 +374,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="15.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>8667695616</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>123456</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{B5B68BFE-B891-405A-8159-CDB3CF776081}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day5-Third commit:The automation implemented appointment booking functionality with confirmation details and manage the booked appointments under My Appointments
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/inputData.xlsx
+++ b/src/test/resources/Exceldata/inputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMILE\Desktop\Apollo Testing\Apollo247TestingApp\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1815D8-DE0B-4C85-A76B-FD2C85007E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139CB665-98C6-4F3F-8CEF-468E4708A2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="2800" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>number</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>abi@gmail.com</t>
+  </si>
+  <si>
+    <t>abi@.com</t>
   </si>
 </sst>
 </file>
@@ -377,7 +380,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,10 +424,14 @@
       <c r="A3">
         <v>123456</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{B5B68BFE-B891-405A-8159-CDB3CF776081}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{B8220B3D-E783-4DFB-B7A1-654F87E912FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Day6-first commit:Verification of failed find doctor scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/inputData.xlsx
+++ b/src/test/resources/Exceldata/inputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMILE\Desktop\Apollo Testing\Apollo247TestingApp\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139CB665-98C6-4F3F-8CEF-468E4708A2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E631AF-E7B9-4C15-AE71-4E02231298E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -380,7 +380,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Day7-first commit:Updation in find doctor
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/inputData.xlsx
+++ b/src/test/resources/Exceldata/inputData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMILE\Desktop\Apollo Testing\Apollo247TestingApp\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E631AF-E7B9-4C15-AE71-4E02231298E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3347F6-0909-4514-8640-256E3F17EF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>number</t>
   </si>
@@ -49,6 +49,21 @@
   </si>
   <si>
     <t>abi@.com</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>other location</t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>newyork</t>
+  </si>
+  <si>
+    <t>Chennai</t>
   </si>
 </sst>
 </file>
@@ -377,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -389,10 +404,11 @@
     <col min="2" max="2" width="13.54296875" customWidth="1"/>
     <col min="3" max="3" width="14.1796875" customWidth="1"/>
     <col min="4" max="4" width="15.08984375" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,8 +421,17 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>8667695616</v>
       </c>
@@ -419,8 +444,17 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>1234567</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>123456</v>
       </c>

</xml_diff>